<commit_message>
remove CM itemtype and 'record' verb
</commit_message>
<xml_diff>
--- a/g6_sample_for_NCME.xlsx
+++ b/g6_sample_for_NCME.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jing.chen/OneDrive - Northwest Evaluation Association/Documents/NWEA/NCME_2022/ItemSpec/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jing.chen/Documents/GitHub/ItemSpec_Automation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5FA1925-A494-3343-8A55-BE49A16C9646}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0D321A9-4DEF-E946-B467-D8112748386F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4600" yWindow="460" windowWidth="37360" windowHeight="19740" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1040" yWindow="2040" windowWidth="37360" windowHeight="19740" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ALL" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="64">
   <si>
     <t>goal</t>
   </si>
@@ -130,9 +130,6 @@
     <t>Orders</t>
   </si>
   <si>
-    <t>Records</t>
-  </si>
-  <si>
     <t>Uses</t>
   </si>
   <si>
@@ -161,9 +158,6 @@
   </si>
   <si>
     <t>Hot Text</t>
-  </si>
-  <si>
-    <t>Multiple Choice or Choice Multiple</t>
   </si>
   <si>
     <t>Gap Match or Graphic Gap Match</t>
@@ -184,59 +178,59 @@
     <t xml:space="preserve">Represents quivalent values for given fractions, decimals, and percents for fractions with denominator greater than 10 (other than 100) or percents that include decimals. </t>
   </si>
   <si>
-    <t xml:space="preserve">Records comparisons of positive numbers (whole numbers, mixed numbers, fractions, and/or decimals to the tenths, hundredths, or thousandths) using symbols. May include a number line. 
+    <t xml:space="preserve">MA 6.1.1.d Convert among fractions, decimals, and percents using multiple representations.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MA 6.1.1.c Compare and order rational numbers both on the number line and not on the number line.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MA 6.1.1.b Represent non-negative whole numbers using exponential notation.
+</t>
+  </si>
+  <si>
+    <t>Explains and justifies a conversion between fractions, decimals, and percents, using symbols, visual models, or other representations.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Converts among fractions and decimals for fractions with denominators of 7 or 9. 
+Converts between percents and fractions  or percents and decimals for whole percents greater than or equal to 1%. </t>
+  </si>
+  <si>
+    <t>To examine in order to note the similarities or differences.</t>
+  </si>
+  <si>
+    <t>To give the meaning or interpretation of; expound; or justify.</t>
+  </si>
+  <si>
+    <t>Select or show an example of a graphic or solution to show conceptual understanding such as selecting or creating a model or more than one algorithm to solve a problem.</t>
+  </si>
+  <si>
+    <t>Uses is often paired with another verb (uses to determine, write, or explain)</t>
+  </si>
+  <si>
+    <t>Change in form.</t>
+  </si>
+  <si>
+    <t>The arrangement of values or symbols in relation to each other according to a particular sequence, pattern, or value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Represents comparisons of positive numbers (whole numbers, mixed numbers, fractions, and/or decimals to the tenths, hundredths, or thousandths) using symbols. May include a number line. 
 Orders three or more positive numbers (whole numbers, mixed numbers, fractions, and/or decimals to the thousandths). May include a number line. 
 Determines what positive number is between two given positive numbers (whole numbers, mixed numbers, fractions, and/or decimals to the thousandths). May include a number line. </t>
   </si>
   <si>
-    <t xml:space="preserve">Uses symbols to represent comparisons between two rational numbers where at least one value is a negative rational number. 
+    <t xml:space="preserve">Represents comparisons between two rational numbers where at least one value is a negative rational number. 
 Orders three or more numbers when at least one value is a negative rational number. </t>
   </si>
   <si>
-    <t xml:space="preserve">Uses symbols to represent comparisons between two rational numbers where at least one value is a decimal to the ten-thousandths or more. 
+    <t xml:space="preserve">Represents comparisons between two rational numbers where at least one value is a decimal to the ten-thousandths or more. 
 Orders three or more positive numbers (whole numbers, mixed numbers, fractions, and/or decimals) with at least one number being a decimal to the ten-thousandths or a percent. 
-Uses symbols to represent comparisons of two rational numbers when at least one value is a negative rational number and both values are plotted on a number line. 
+Represents comparisons of two rational numbers when at least one value is a negative rational number and both values are plotted on a number line. 
 Orders three rational numbers on a number line when at least one value is a negative rational number. </t>
   </si>
   <si>
-    <t xml:space="preserve">MA 6.1.1.d Convert among fractions, decimals, and percents using multiple representations.
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MA 6.1.1.c Compare and order rational numbers both on the number line and not on the number line.
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MA 6.1.1.b Represent non-negative whole numbers using exponential notation.
-</t>
-  </si>
-  <si>
-    <t>Explains and justifies a conversion between fractions, decimals, and percents, using symbols, visual models, or other representations.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Converts among fractions and decimals for fractions with denominators of 7 or 9. 
-Converts between percents and fractions  or percents and decimals for whole percents greater than or equal to 1%. </t>
-  </si>
-  <si>
-    <t>To examine in order to note the similarities or differences.</t>
-  </si>
-  <si>
-    <t>To give the meaning or interpretation of; expound; or justify.</t>
-  </si>
-  <si>
-    <t>Select or show an example of a graphic or solution to show conceptual understanding such as selecting or creating a model or more than one algorithm to solve a problem.</t>
-  </si>
-  <si>
-    <t>Uses is often paired with another verb (uses to determine, write, or explain)</t>
-  </si>
-  <si>
-    <t>Change in form.</t>
-  </si>
-  <si>
-    <t>The arrangement of values or symbols in relation to each other according to a particular sequence, pattern, or value</t>
-  </si>
-  <si>
-    <t>Set down in writing or some other form.</t>
+    <t>Multiple Choice</t>
   </si>
 </sst>
 </file>
@@ -309,7 +303,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -332,12 +326,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -683,8 +671,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L5"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView topLeftCell="E3" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -791,16 +779,16 @@
         <v>15</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="G3" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="I3" s="2" t="s">
         <v>47</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>49</v>
       </c>
       <c r="J3" s="2">
         <v>1</v>
@@ -829,16 +817,16 @@
         <v>15</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>52</v>
+        <v>61</v>
       </c>
       <c r="J4" s="2">
         <v>2</v>
@@ -867,16 +855,16 @@
         <v>15</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="J5">
         <v>1</v>
@@ -895,10 +883,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E2E6D36-AB23-5942-A24B-B397307C9EB2}">
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+      <selection activeCell="H15" sqref="H15:H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -907,30 +895,30 @@
     <col min="9" max="9" width="37" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="64" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" ht="48" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>20</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="F1" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="H1" s="3" t="s">
         <v>42</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>43</v>
       </c>
       <c r="I1" s="3" t="s">
         <v>29</v>
@@ -960,26 +948,26 @@
         <v>21</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" s="10" t="s">
-        <v>36</v>
+      <c r="A3" s="7" t="s">
+        <v>35</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="8"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="H3" s="11" t="s">
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="H3" s="9" t="s">
         <v>21</v>
       </c>
       <c r="I3" s="6" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="16" x14ac:dyDescent="0.2">
@@ -1002,7 +990,7 @@
         <v>21</v>
       </c>
       <c r="I4" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:9" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
@@ -1025,7 +1013,7 @@
         <v>21</v>
       </c>
       <c r="I5" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="16" x14ac:dyDescent="0.2">
@@ -1050,7 +1038,7 @@
       </c>
       <c r="H6" s="8"/>
       <c r="I6" s="6" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="13" customHeight="1" x14ac:dyDescent="0.2">
@@ -1069,54 +1057,64 @@
       </c>
       <c r="H7" s="8"/>
       <c r="I7" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A8" s="10" t="s">
+      <c r="A8" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="C8" s="11"/>
+      <c r="C8" s="9"/>
       <c r="D8" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="E8" s="11"/>
-      <c r="F8" s="11"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9"/>
       <c r="G8" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="H8" s="11"/>
+      <c r="H8" s="9"/>
       <c r="I8" s="6" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A9" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="I9" s="9" t="s">
-        <v>65</v>
+      <c r="A9" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="G9" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="H9" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="I9" s="6" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="B10" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="C10" s="8"/>
+      <c r="C10" s="8" t="s">
+        <v>21</v>
+      </c>
       <c r="D10" s="8" t="s">
         <v>21</v>
       </c>
@@ -1133,41 +1131,12 @@
         <v>21</v>
       </c>
       <c r="I10" s="6" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A11" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="B11" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="C11" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="D11" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="E11" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="F11" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="G11" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="H11" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="I11" s="6" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I11">
-    <sortCondition ref="A2:A11"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I10">
+    <sortCondition ref="A2:A10"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>